<commit_message>
I2C master and slave update
I2C slave 仍不穩定
</commit_message>
<xml_diff>
--- a/doc/I2C_COMMAND.xlsx
+++ b/doc/I2C_COMMAND.xlsx
@@ -16,19 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
-  <si>
-    <t>@A0#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Action</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>input</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>return</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -37,14 +30,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set display</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Read key</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -53,10 +38,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Write EEPROM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Firmware version</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -65,173 +46,219 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>@WELCOME\0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>for test</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@VERXXXXXXXX\0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>LED current</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>@A5X#</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A5X\0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A2X#</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A2YY\0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X: 0 -&gt; once, 1 -&gt; continuous
-YY: key status, 8 bit
+    <t>Led flash control</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01 '1' '2' '3': display"123"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">X X X </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>03</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>N X</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>04</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X Y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read test buffer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write test buffer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write N X to 03H first, then read 03H
+@A3700# : read EEPROM from address 00 to 06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">04 01 A5 : write EEPROM address 0x01 with data 0xA5
+Note: 5ms between successive write </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write N X to 03H first, then read 03H
+@A3700# : read buffer from address 00 to 06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>04 01 A5 : write buffer address 0x01 with data 0xA5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write EEPROM
+(one byte)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X: 7 segment display, '0'~'F'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write EEPROM
+(bytes)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">X1 X2 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>02 03 E7: display"999"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X1X2: height(16 bits), X1 is MSB
+0000 ~ 03E7</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set display
+(string)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y: key status, 8 bit
 bit    7 6  5  4  3  2  1  0
 -----------------------------
 key    0 S7 S6 S5 S4 S3 S2 S1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>@B0#</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Led flash control</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A6XXXXYYYY#</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A6XXXXYYYY\0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>XXXX:duty,0000~9999 
-YYYY:Period, 0000~9999
+    <t>20</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXXXXXXX</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X1 X2 Y1 Y2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X1 X2:duty,16 bits, X1 is MSB
+Y1 Y2:Period, 16 bits, Y1 is MSB
 1 sec = 1953</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">X:0~3   </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A51# : set led current level to 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A608001600: set display flash at 50% duty</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>@A20# : read key one time
-@A21# : read key continuous</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>01 '1' '2' '3': display"123"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">X X X </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X: 7 segment display, 0~F</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>03</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>N X</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y Y Y Y Y Y …</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write N X to 03H first, then read 03H
-@A3700# : read EEPROM from address 00 to 06</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X:Start address 
-N:number of bytes(n&lt;=7)
+    <t>21 03 E8 07 D0: set display flash at 50% duty, period is about 1 sec</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X:0~3   4mA, 7mA, 10mA, 12mA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set display
+(number)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>parameters</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X:address, 00~3F 
 Y:data</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Read Status</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>02</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>04</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>05</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>06</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit 0: Read EEPROM data ready</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X Y</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X:address, 00~3F Y:data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>04 01 A5 : write EEPROM address 0x01 with data 0xA5</t>
+    <t>X:address, 00~3F  
+N:number of bytes(n&lt;=16)
+Y:data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>N X Y1 Y2 .. Yn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1 Y2 … Yn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X:address, 00~3F  
+N:number of bytes(n&lt;=16)
+Y:data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X:address, 0~7  
+N:number of bytes(n&lt;=16)
+Y:data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X:address, 0~7 Y:data</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -662,10 +689,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:F16"/>
+  <dimension ref="A3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -680,203 +707,217 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="31.5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="78.75">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="58.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="31.5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="47.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="47.25" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="63">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="47.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58.5" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="4" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="31.5">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="47.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="58.5" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
@@ -893,6 +934,22 @@
       <c r="D16" s="4"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>